<commit_message>
Súlyozott map, known error: ha sarokjárdára kell menni
</commit_message>
<xml_diff>
--- a/Other/map.xlsx
+++ b/Other/map.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C98052-EC61-41C8-A2BB-2BCD0D14731A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B5C65D-D607-4F95-8F45-0B195007023F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3660" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3660" uniqueCount="67">
   <si>
     <t>G</t>
   </si>
@@ -231,6 +231,9 @@
   <si>
     <t>Oszlop60</t>
   </si>
+  <si>
+    <t>K</t>
+  </si>
 </sst>
 </file>
 
@@ -348,7 +351,7 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="69">
     <dxf>
       <fill>
         <patternFill>
@@ -367,211 +370,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -789,32 +587,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
+          <bgColor theme="5" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -901,69 +676,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E10DE2FA-2DD2-4EBF-BD63-DCCFA5FF4AD0}" name="Új_szöveges_dokumentum__2" displayName="Új_szöveges_dokumentum__2" ref="B2:BI63" tableType="queryTable" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E10DE2FA-2DD2-4EBF-BD63-DCCFA5FF4AD0}" name="Új_szöveges_dokumentum__2" displayName="Új_szöveges_dokumentum__2" ref="B2:BI63" tableType="queryTable" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="B2:BI63" xr:uid="{DE6A2C29-F277-44C9-8C93-967D97F43468}"/>
   <tableColumns count="60">
-    <tableColumn id="1" xr3:uid="{571AD5BC-C083-42BF-B574-6B0FBB157DF0}" uniqueName="1" name="Oszlop1" queryTableFieldId="1" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{C9DF9092-1CA9-40C8-A22F-7A8869D9424A}" uniqueName="2" name="Oszlop2" queryTableFieldId="2" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{1940D9A0-FA6D-450E-954A-327328FAD826}" uniqueName="3" name="Oszlop3" queryTableFieldId="3" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{2A5ED6A7-336E-4B7D-A3AC-98F46318660C}" uniqueName="4" name="Oszlop4" queryTableFieldId="4" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{C46B2876-075E-4A8F-9B7F-C00ED18EDD9E}" uniqueName="5" name="Oszlop5" queryTableFieldId="5" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{FE8BB0FA-E307-41D5-A4D5-83BC407B483B}" uniqueName="6" name="Oszlop6" queryTableFieldId="6" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{CF838701-4A2F-48D0-B9C6-412E40976BE5}" uniqueName="7" name="Oszlop7" queryTableFieldId="7" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{AD5E97A2-8DFF-4FDD-99FB-198BCC791896}" uniqueName="8" name="Oszlop8" queryTableFieldId="8" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{002787B7-36A3-48F0-A0FB-EAB79DED4A47}" uniqueName="9" name="Oszlop9" queryTableFieldId="9" dataDxfId="84"/>
-    <tableColumn id="10" xr3:uid="{DFC565FE-8C60-4884-8FFE-CC9333AF9395}" uniqueName="10" name="Oszlop10" queryTableFieldId="10" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{722E9B4E-06E4-41C4-8B7E-6FAF204EB181}" uniqueName="11" name="Oszlop11" queryTableFieldId="11" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{38A759ED-503A-4B6B-9F64-9079BC4F39FB}" uniqueName="12" name="Oszlop12" queryTableFieldId="12" dataDxfId="81"/>
-    <tableColumn id="13" xr3:uid="{1AC73B55-C9E0-43D0-A7BF-202C3671673B}" uniqueName="13" name="Oszlop13" queryTableFieldId="13" dataDxfId="80"/>
-    <tableColumn id="14" xr3:uid="{417BBF16-E3DA-4647-A97B-373B730DD852}" uniqueName="14" name="Oszlop14" queryTableFieldId="14" dataDxfId="79"/>
-    <tableColumn id="15" xr3:uid="{D4986906-906C-4AB4-B937-29D30057A671}" uniqueName="15" name="Oszlop15" queryTableFieldId="15" dataDxfId="78"/>
-    <tableColumn id="16" xr3:uid="{78CBD81C-A1B7-4932-B9FB-CACB8AE58870}" uniqueName="16" name="Oszlop16" queryTableFieldId="16" dataDxfId="77"/>
-    <tableColumn id="17" xr3:uid="{54C14E6E-6902-4E6B-8AE9-4B3166DB4547}" uniqueName="17" name="Oszlop17" queryTableFieldId="17" dataDxfId="76"/>
-    <tableColumn id="18" xr3:uid="{F0CF5061-6D60-476A-9917-BB304D5B2F3B}" uniqueName="18" name="Oszlop18" queryTableFieldId="18" dataDxfId="75"/>
-    <tableColumn id="19" xr3:uid="{B7ED95A7-7731-4BDD-B716-EAB0B8ADC13C}" uniqueName="19" name="Oszlop19" queryTableFieldId="19" dataDxfId="74"/>
-    <tableColumn id="20" xr3:uid="{2642BBD0-6B3B-4AC3-8E46-6AEFC98F6BF8}" uniqueName="20" name="Oszlop20" queryTableFieldId="20" dataDxfId="73"/>
-    <tableColumn id="21" xr3:uid="{A7CAB78C-7F7D-4125-8C83-844AD8BBF589}" uniqueName="21" name="Oszlop21" queryTableFieldId="21" dataDxfId="72"/>
-    <tableColumn id="22" xr3:uid="{C14EAE52-E574-4B5D-A1D3-BFD493B98DBE}" uniqueName="22" name="Oszlop22" queryTableFieldId="22" dataDxfId="71"/>
-    <tableColumn id="23" xr3:uid="{13582685-CA33-47C4-9CCB-6D9A7F52C43D}" uniqueName="23" name="Oszlop23" queryTableFieldId="23" dataDxfId="70"/>
-    <tableColumn id="24" xr3:uid="{6FFB97CC-6E70-4E82-9D90-EE0C180FBCFC}" uniqueName="24" name="Oszlop24" queryTableFieldId="24" dataDxfId="69"/>
-    <tableColumn id="25" xr3:uid="{91ED95D3-C1A0-41EB-AB8B-59048DD3F413}" uniqueName="25" name="Oszlop25" queryTableFieldId="25" dataDxfId="68"/>
-    <tableColumn id="26" xr3:uid="{A8EE2F7E-EFAB-4814-A201-71210F714BD6}" uniqueName="26" name="Oszlop26" queryTableFieldId="26" dataDxfId="67"/>
-    <tableColumn id="27" xr3:uid="{2C247694-0122-485F-9BE1-43873B9E2424}" uniqueName="27" name="Oszlop27" queryTableFieldId="27" dataDxfId="66"/>
-    <tableColumn id="28" xr3:uid="{2EC2FDCC-202F-4CF5-9841-4489828FA291}" uniqueName="28" name="Oszlop28" queryTableFieldId="28" dataDxfId="65"/>
-    <tableColumn id="29" xr3:uid="{D8947960-AC94-422C-A2E7-D39E56BDE2A4}" uniqueName="29" name="Oszlop29" queryTableFieldId="29" dataDxfId="64"/>
-    <tableColumn id="30" xr3:uid="{14352C38-138F-4075-B0CA-43086B5A7555}" uniqueName="30" name="Oszlop30" queryTableFieldId="30" dataDxfId="63"/>
-    <tableColumn id="31" xr3:uid="{EEF32F65-3DD5-4178-BE9A-871DDCA74D6C}" uniqueName="31" name="Oszlop31" queryTableFieldId="31" dataDxfId="62"/>
-    <tableColumn id="32" xr3:uid="{87798D8B-1A70-4A54-B13D-9F7FDB265EAB}" uniqueName="32" name="Oszlop32" queryTableFieldId="32" dataDxfId="61"/>
-    <tableColumn id="33" xr3:uid="{A039D294-2C3C-4282-89EC-CA945937FC89}" uniqueName="33" name="Oszlop33" queryTableFieldId="33" dataDxfId="60"/>
-    <tableColumn id="34" xr3:uid="{558BEDC9-76B9-4880-8347-5ACE25A74D4B}" uniqueName="34" name="Oszlop34" queryTableFieldId="34" dataDxfId="59"/>
-    <tableColumn id="35" xr3:uid="{32F6F95F-646E-451D-8204-1CA6125D422E}" uniqueName="35" name="Oszlop35" queryTableFieldId="35" dataDxfId="58"/>
-    <tableColumn id="36" xr3:uid="{5FA7C415-5357-44C3-8261-93E9E0756229}" uniqueName="36" name="Oszlop36" queryTableFieldId="36" dataDxfId="57"/>
-    <tableColumn id="37" xr3:uid="{D1EC40EC-AB47-4892-BC89-CE2489FCC7EC}" uniqueName="37" name="Oszlop37" queryTableFieldId="37" dataDxfId="56"/>
-    <tableColumn id="38" xr3:uid="{C660067B-ECD9-417D-8C7F-0D0FB927B147}" uniqueName="38" name="Oszlop38" queryTableFieldId="38" dataDxfId="55"/>
-    <tableColumn id="39" xr3:uid="{D8CEFF35-9BAC-4746-95F5-2FF0D0BBC54F}" uniqueName="39" name="Oszlop39" queryTableFieldId="39" dataDxfId="54"/>
-    <tableColumn id="40" xr3:uid="{94399687-0669-4E77-B1A5-0983E8273F84}" uniqueName="40" name="Oszlop40" queryTableFieldId="40" dataDxfId="53"/>
-    <tableColumn id="41" xr3:uid="{819C45A2-EFCD-43D5-AAA8-A165D044725D}" uniqueName="41" name="Oszlop41" queryTableFieldId="41" dataDxfId="52"/>
-    <tableColumn id="42" xr3:uid="{5D4F8E08-F532-4989-856B-5D53A877502A}" uniqueName="42" name="Oszlop42" queryTableFieldId="42" dataDxfId="51"/>
-    <tableColumn id="43" xr3:uid="{043A2811-1D13-4503-8E97-0ED410BEED4D}" uniqueName="43" name="Oszlop43" queryTableFieldId="43" dataDxfId="50"/>
-    <tableColumn id="44" xr3:uid="{62485A93-DE05-464F-80AD-8C33624E942A}" uniqueName="44" name="Oszlop44" queryTableFieldId="44" dataDxfId="49"/>
-    <tableColumn id="45" xr3:uid="{01708938-DD66-4F24-8BFF-0E1F1DDAD074}" uniqueName="45" name="Oszlop45" queryTableFieldId="45" dataDxfId="48"/>
-    <tableColumn id="46" xr3:uid="{3BEAEB2C-0578-4DF3-A9E0-62916847D26D}" uniqueName="46" name="Oszlop46" queryTableFieldId="46" dataDxfId="47"/>
-    <tableColumn id="47" xr3:uid="{E485321B-FF02-4BC2-AA5F-2DAF24FFB9E8}" uniqueName="47" name="Oszlop47" queryTableFieldId="47" dataDxfId="46"/>
-    <tableColumn id="48" xr3:uid="{F207BB99-37CB-4B54-923D-7608710A3094}" uniqueName="48" name="Oszlop48" queryTableFieldId="48" dataDxfId="45"/>
-    <tableColumn id="49" xr3:uid="{9C7308CF-7867-49EE-B044-C4A6A880B801}" uniqueName="49" name="Oszlop49" queryTableFieldId="49" dataDxfId="44"/>
-    <tableColumn id="50" xr3:uid="{6633743B-BD5B-4680-B85A-BEEB9268A167}" uniqueName="50" name="Oszlop50" queryTableFieldId="50" dataDxfId="43"/>
-    <tableColumn id="51" xr3:uid="{7CBC244D-621B-4B5C-BFC5-080808480784}" uniqueName="51" name="Oszlop51" queryTableFieldId="51" dataDxfId="42"/>
-    <tableColumn id="52" xr3:uid="{2672080F-A2C0-449E-B978-572D6C71ACAA}" uniqueName="52" name="Oszlop52" queryTableFieldId="52" dataDxfId="41"/>
-    <tableColumn id="53" xr3:uid="{7398282F-4BD3-4F19-80EE-83F55CD8941B}" uniqueName="53" name="Oszlop53" queryTableFieldId="53" dataDxfId="40"/>
-    <tableColumn id="54" xr3:uid="{7EC70838-1EBA-4E85-A4D1-97EAAE14C8CB}" uniqueName="54" name="Oszlop54" queryTableFieldId="54" dataDxfId="39"/>
-    <tableColumn id="55" xr3:uid="{24B25E3D-B137-4097-A429-FEF53AACE908}" uniqueName="55" name="Oszlop55" queryTableFieldId="55" dataDxfId="38"/>
-    <tableColumn id="56" xr3:uid="{E26C030B-063B-4400-B43B-DDBD3C4325FC}" uniqueName="56" name="Oszlop56" queryTableFieldId="56" dataDxfId="37"/>
-    <tableColumn id="57" xr3:uid="{F23F0C29-A916-493F-9C3A-E0522BA1C6F3}" uniqueName="57" name="Oszlop57" queryTableFieldId="57" dataDxfId="36"/>
-    <tableColumn id="58" xr3:uid="{5C492DC9-2A1E-4512-A4FA-4B5F49DB562A}" uniqueName="58" name="Oszlop58" queryTableFieldId="58" dataDxfId="35"/>
-    <tableColumn id="59" xr3:uid="{0879E9F1-DA9E-4FC9-91DD-80A87E3762FE}" uniqueName="59" name="Oszlop59" queryTableFieldId="59" dataDxfId="34"/>
-    <tableColumn id="60" xr3:uid="{DC997E2C-B6E3-43E5-8E8F-BFA01D35DAA7}" uniqueName="60" name="Oszlop60" queryTableFieldId="60" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{571AD5BC-C083-42BF-B574-6B0FBB157DF0}" uniqueName="1" name="Oszlop1" queryTableFieldId="1" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{C9DF9092-1CA9-40C8-A22F-7A8869D9424A}" uniqueName="2" name="Oszlop2" queryTableFieldId="2" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{1940D9A0-FA6D-450E-954A-327328FAD826}" uniqueName="3" name="Oszlop3" queryTableFieldId="3" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{2A5ED6A7-336E-4B7D-A3AC-98F46318660C}" uniqueName="4" name="Oszlop4" queryTableFieldId="4" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{C46B2876-075E-4A8F-9B7F-C00ED18EDD9E}" uniqueName="5" name="Oszlop5" queryTableFieldId="5" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{FE8BB0FA-E307-41D5-A4D5-83BC407B483B}" uniqueName="6" name="Oszlop6" queryTableFieldId="6" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{CF838701-4A2F-48D0-B9C6-412E40976BE5}" uniqueName="7" name="Oszlop7" queryTableFieldId="7" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{AD5E97A2-8DFF-4FDD-99FB-198BCC791896}" uniqueName="8" name="Oszlop8" queryTableFieldId="8" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{002787B7-36A3-48F0-A0FB-EAB79DED4A47}" uniqueName="9" name="Oszlop9" queryTableFieldId="9" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{DFC565FE-8C60-4884-8FFE-CC9333AF9395}" uniqueName="10" name="Oszlop10" queryTableFieldId="10" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{722E9B4E-06E4-41C4-8B7E-6FAF204EB181}" uniqueName="11" name="Oszlop11" queryTableFieldId="11" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{38A759ED-503A-4B6B-9F64-9079BC4F39FB}" uniqueName="12" name="Oszlop12" queryTableFieldId="12" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{1AC73B55-C9E0-43D0-A7BF-202C3671673B}" uniqueName="13" name="Oszlop13" queryTableFieldId="13" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{417BBF16-E3DA-4647-A97B-373B730DD852}" uniqueName="14" name="Oszlop14" queryTableFieldId="14" dataDxfId="52"/>
+    <tableColumn id="15" xr3:uid="{D4986906-906C-4AB4-B937-29D30057A671}" uniqueName="15" name="Oszlop15" queryTableFieldId="15" dataDxfId="51"/>
+    <tableColumn id="16" xr3:uid="{78CBD81C-A1B7-4932-B9FB-CACB8AE58870}" uniqueName="16" name="Oszlop16" queryTableFieldId="16" dataDxfId="50"/>
+    <tableColumn id="17" xr3:uid="{54C14E6E-6902-4E6B-8AE9-4B3166DB4547}" uniqueName="17" name="Oszlop17" queryTableFieldId="17" dataDxfId="49"/>
+    <tableColumn id="18" xr3:uid="{F0CF5061-6D60-476A-9917-BB304D5B2F3B}" uniqueName="18" name="Oszlop18" queryTableFieldId="18" dataDxfId="48"/>
+    <tableColumn id="19" xr3:uid="{B7ED95A7-7731-4BDD-B716-EAB0B8ADC13C}" uniqueName="19" name="Oszlop19" queryTableFieldId="19" dataDxfId="47"/>
+    <tableColumn id="20" xr3:uid="{2642BBD0-6B3B-4AC3-8E46-6AEFC98F6BF8}" uniqueName="20" name="Oszlop20" queryTableFieldId="20" dataDxfId="46"/>
+    <tableColumn id="21" xr3:uid="{A7CAB78C-7F7D-4125-8C83-844AD8BBF589}" uniqueName="21" name="Oszlop21" queryTableFieldId="21" dataDxfId="45"/>
+    <tableColumn id="22" xr3:uid="{C14EAE52-E574-4B5D-A1D3-BFD493B98DBE}" uniqueName="22" name="Oszlop22" queryTableFieldId="22" dataDxfId="44"/>
+    <tableColumn id="23" xr3:uid="{13582685-CA33-47C4-9CCB-6D9A7F52C43D}" uniqueName="23" name="Oszlop23" queryTableFieldId="23" dataDxfId="43"/>
+    <tableColumn id="24" xr3:uid="{6FFB97CC-6E70-4E82-9D90-EE0C180FBCFC}" uniqueName="24" name="Oszlop24" queryTableFieldId="24" dataDxfId="42"/>
+    <tableColumn id="25" xr3:uid="{91ED95D3-C1A0-41EB-AB8B-59048DD3F413}" uniqueName="25" name="Oszlop25" queryTableFieldId="25" dataDxfId="41"/>
+    <tableColumn id="26" xr3:uid="{A8EE2F7E-EFAB-4814-A201-71210F714BD6}" uniqueName="26" name="Oszlop26" queryTableFieldId="26" dataDxfId="40"/>
+    <tableColumn id="27" xr3:uid="{2C247694-0122-485F-9BE1-43873B9E2424}" uniqueName="27" name="Oszlop27" queryTableFieldId="27" dataDxfId="39"/>
+    <tableColumn id="28" xr3:uid="{2EC2FDCC-202F-4CF5-9841-4489828FA291}" uniqueName="28" name="Oszlop28" queryTableFieldId="28" dataDxfId="38"/>
+    <tableColumn id="29" xr3:uid="{D8947960-AC94-422C-A2E7-D39E56BDE2A4}" uniqueName="29" name="Oszlop29" queryTableFieldId="29" dataDxfId="37"/>
+    <tableColumn id="30" xr3:uid="{14352C38-138F-4075-B0CA-43086B5A7555}" uniqueName="30" name="Oszlop30" queryTableFieldId="30" dataDxfId="36"/>
+    <tableColumn id="31" xr3:uid="{EEF32F65-3DD5-4178-BE9A-871DDCA74D6C}" uniqueName="31" name="Oszlop31" queryTableFieldId="31" dataDxfId="35"/>
+    <tableColumn id="32" xr3:uid="{87798D8B-1A70-4A54-B13D-9F7FDB265EAB}" uniqueName="32" name="Oszlop32" queryTableFieldId="32" dataDxfId="34"/>
+    <tableColumn id="33" xr3:uid="{A039D294-2C3C-4282-89EC-CA945937FC89}" uniqueName="33" name="Oszlop33" queryTableFieldId="33" dataDxfId="33"/>
+    <tableColumn id="34" xr3:uid="{558BEDC9-76B9-4880-8347-5ACE25A74D4B}" uniqueName="34" name="Oszlop34" queryTableFieldId="34" dataDxfId="32"/>
+    <tableColumn id="35" xr3:uid="{32F6F95F-646E-451D-8204-1CA6125D422E}" uniqueName="35" name="Oszlop35" queryTableFieldId="35" dataDxfId="31"/>
+    <tableColumn id="36" xr3:uid="{5FA7C415-5357-44C3-8261-93E9E0756229}" uniqueName="36" name="Oszlop36" queryTableFieldId="36" dataDxfId="30"/>
+    <tableColumn id="37" xr3:uid="{D1EC40EC-AB47-4892-BC89-CE2489FCC7EC}" uniqueName="37" name="Oszlop37" queryTableFieldId="37" dataDxfId="29"/>
+    <tableColumn id="38" xr3:uid="{C660067B-ECD9-417D-8C7F-0D0FB927B147}" uniqueName="38" name="Oszlop38" queryTableFieldId="38" dataDxfId="28"/>
+    <tableColumn id="39" xr3:uid="{D8CEFF35-9BAC-4746-95F5-2FF0D0BBC54F}" uniqueName="39" name="Oszlop39" queryTableFieldId="39" dataDxfId="27"/>
+    <tableColumn id="40" xr3:uid="{94399687-0669-4E77-B1A5-0983E8273F84}" uniqueName="40" name="Oszlop40" queryTableFieldId="40" dataDxfId="26"/>
+    <tableColumn id="41" xr3:uid="{819C45A2-EFCD-43D5-AAA8-A165D044725D}" uniqueName="41" name="Oszlop41" queryTableFieldId="41" dataDxfId="25"/>
+    <tableColumn id="42" xr3:uid="{5D4F8E08-F532-4989-856B-5D53A877502A}" uniqueName="42" name="Oszlop42" queryTableFieldId="42" dataDxfId="24"/>
+    <tableColumn id="43" xr3:uid="{043A2811-1D13-4503-8E97-0ED410BEED4D}" uniqueName="43" name="Oszlop43" queryTableFieldId="43" dataDxfId="23"/>
+    <tableColumn id="44" xr3:uid="{62485A93-DE05-464F-80AD-8C33624E942A}" uniqueName="44" name="Oszlop44" queryTableFieldId="44" dataDxfId="22"/>
+    <tableColumn id="45" xr3:uid="{01708938-DD66-4F24-8BFF-0E1F1DDAD074}" uniqueName="45" name="Oszlop45" queryTableFieldId="45" dataDxfId="21"/>
+    <tableColumn id="46" xr3:uid="{3BEAEB2C-0578-4DF3-A9E0-62916847D26D}" uniqueName="46" name="Oszlop46" queryTableFieldId="46" dataDxfId="20"/>
+    <tableColumn id="47" xr3:uid="{E485321B-FF02-4BC2-AA5F-2DAF24FFB9E8}" uniqueName="47" name="Oszlop47" queryTableFieldId="47" dataDxfId="19"/>
+    <tableColumn id="48" xr3:uid="{F207BB99-37CB-4B54-923D-7608710A3094}" uniqueName="48" name="Oszlop48" queryTableFieldId="48" dataDxfId="18"/>
+    <tableColumn id="49" xr3:uid="{9C7308CF-7867-49EE-B044-C4A6A880B801}" uniqueName="49" name="Oszlop49" queryTableFieldId="49" dataDxfId="17"/>
+    <tableColumn id="50" xr3:uid="{6633743B-BD5B-4680-B85A-BEEB9268A167}" uniqueName="50" name="Oszlop50" queryTableFieldId="50" dataDxfId="16"/>
+    <tableColumn id="51" xr3:uid="{7CBC244D-621B-4B5C-BFC5-080808480784}" uniqueName="51" name="Oszlop51" queryTableFieldId="51" dataDxfId="15"/>
+    <tableColumn id="52" xr3:uid="{2672080F-A2C0-449E-B978-572D6C71ACAA}" uniqueName="52" name="Oszlop52" queryTableFieldId="52" dataDxfId="14"/>
+    <tableColumn id="53" xr3:uid="{7398282F-4BD3-4F19-80EE-83F55CD8941B}" uniqueName="53" name="Oszlop53" queryTableFieldId="53" dataDxfId="13"/>
+    <tableColumn id="54" xr3:uid="{7EC70838-1EBA-4E85-A4D1-97EAAE14C8CB}" uniqueName="54" name="Oszlop54" queryTableFieldId="54" dataDxfId="12"/>
+    <tableColumn id="55" xr3:uid="{24B25E3D-B137-4097-A429-FEF53AACE908}" uniqueName="55" name="Oszlop55" queryTableFieldId="55" dataDxfId="11"/>
+    <tableColumn id="56" xr3:uid="{E26C030B-063B-4400-B43B-DDBD3C4325FC}" uniqueName="56" name="Oszlop56" queryTableFieldId="56" dataDxfId="10"/>
+    <tableColumn id="57" xr3:uid="{F23F0C29-A916-493F-9C3A-E0522BA1C6F3}" uniqueName="57" name="Oszlop57" queryTableFieldId="57" dataDxfId="9"/>
+    <tableColumn id="58" xr3:uid="{5C492DC9-2A1E-4512-A4FA-4B5F49DB562A}" uniqueName="58" name="Oszlop58" queryTableFieldId="58" dataDxfId="8"/>
+    <tableColumn id="59" xr3:uid="{0879E9F1-DA9E-4FC9-91DD-80A87E3762FE}" uniqueName="59" name="Oszlop59" queryTableFieldId="59" dataDxfId="7"/>
+    <tableColumn id="60" xr3:uid="{DC997E2C-B6E3-43E5-8E8F-BFA01D35DAA7}" uniqueName="60" name="Oszlop60" queryTableFieldId="60" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1234,18 +1009,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554198ED-48BB-4219-B73C-9BDA64B3C366}">
   <dimension ref="A1:BJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="61" width="3.7109375" style="1" customWidth="1"/>
+    <col min="1" max="61" width="3.6640625" style="1" customWidth="1"/>
     <col min="62" max="62" width="4" style="1" customWidth="1"/>
-    <col min="63" max="16384" width="9.140625" style="1"/>
+    <col min="63" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>0</v>
       </c>
@@ -1433,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1617,7 +1392,7 @@
       </c>
       <c r="BJ2" s="3"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1805,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1993,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2181,7 +1956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2369,7 +2144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2557,7 +2332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2745,7 +2520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2933,7 +2708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -3121,7 +2896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -3309,7 +3084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -3497,7 +3272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -3523,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>1</v>
@@ -3685,7 +3460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -3711,16 +3486,16 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>1</v>
@@ -3873,7 +3648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -3902,16 +3677,16 @@
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>1</v>
@@ -4061,7 +3836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -4093,16 +3868,16 @@
         <v>1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>1</v>
@@ -4249,7 +4024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -4284,16 +4059,16 @@
         <v>1</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>1</v>
@@ -4437,7 +4212,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -4475,13 +4250,13 @@
         <v>1</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>2</v>
@@ -4547,7 +4322,7 @@
         <v>2</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL18" s="1" t="s">
         <v>1</v>
@@ -4625,7 +4400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -4666,10 +4441,10 @@
         <v>1</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>2</v>
@@ -4735,13 +4510,13 @@
         <v>1</v>
       </c>
       <c r="AK19" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL19" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM19" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN19" s="1" t="s">
         <v>1</v>
@@ -4813,7 +4588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -4917,22 +4692,22 @@
         <v>1</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AJ20" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AK20" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL20" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM20" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN20" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO20" s="1" t="s">
         <v>1</v>
@@ -5001,7 +4776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -5105,7 +4880,7 @@
         <v>2</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AJ21" s="1" t="s">
         <v>1</v>
@@ -5114,16 +4889,16 @@
         <v>1</v>
       </c>
       <c r="AL21" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM21" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN21" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO21" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AP21" s="1" t="s">
         <v>1</v>
@@ -5189,7 +4964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -5305,16 +5080,16 @@
         <v>1</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO22" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AP22" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AQ22" s="1" t="s">
         <v>1</v>
@@ -5377,7 +5152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -5487,7 +5262,7 @@
         <v>2</v>
       </c>
       <c r="AK23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL23" s="1" t="s">
         <v>1</v>
@@ -5496,16 +5271,16 @@
         <v>1</v>
       </c>
       <c r="AN23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AP23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AQ23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR23" s="1" t="s">
         <v>1</v>
@@ -5517,10 +5292,10 @@
         <v>1</v>
       </c>
       <c r="AU23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV23" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AW23" s="1" t="s">
         <v>2</v>
@@ -5565,7 +5340,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -5675,10 +5450,10 @@
         <v>2</v>
       </c>
       <c r="AK24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM24" s="1" t="s">
         <v>1</v>
@@ -5687,31 +5462,31 @@
         <v>1</v>
       </c>
       <c r="AO24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AP24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AQ24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AS24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AT24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AU24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AW24" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AX24" s="1" t="s">
         <v>1</v>
@@ -5753,7 +5528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -5860,16 +5635,16 @@
         <v>1</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AK25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN25" s="1" t="s">
         <v>1</v>
@@ -5878,25 +5653,25 @@
         <v>1</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AQ25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AT25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AU25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV25" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AW25" s="1" t="s">
         <v>1</v>
@@ -5941,7 +5716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -6051,16 +5826,16 @@
         <v>1</v>
       </c>
       <c r="AK26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AL26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO26" s="1" t="s">
         <v>1</v>
@@ -6069,19 +5844,19 @@
         <v>1</v>
       </c>
       <c r="AQ26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AS26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AT26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AU26" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV26" s="1" t="s">
         <v>1</v>
@@ -6129,7 +5904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -6242,16 +6017,16 @@
         <v>1</v>
       </c>
       <c r="AL27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AM27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AP27" s="1" t="s">
         <v>1</v>
@@ -6266,13 +6041,13 @@
         <v>1</v>
       </c>
       <c r="AT27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AU27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV27" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AW27" s="1" t="s">
         <v>1</v>
@@ -6317,7 +6092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -6433,13 +6208,13 @@
         <v>1</v>
       </c>
       <c r="AM28" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AN28" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO28" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AP28" s="1" t="s">
         <v>2</v>
@@ -6454,10 +6229,10 @@
         <v>1</v>
       </c>
       <c r="AT28" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AU28" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV28" s="1" t="s">
         <v>2</v>
@@ -6505,7 +6280,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -6624,7 +6399,7 @@
         <v>1</v>
       </c>
       <c r="AN29" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AO29" s="1" t="s">
         <v>2</v>
@@ -6645,7 +6420,7 @@
         <v>1</v>
       </c>
       <c r="AU29" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AV29" s="1" t="s">
         <v>2</v>
@@ -6693,7 +6468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -6881,7 +6656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -7069,7 +6844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -7257,7 +7032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -7445,7 +7220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -7510,10 +7285,10 @@
         <v>1</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="X34" s="1" t="s">
         <v>1</v>
@@ -7633,7 +7408,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -7665,10 +7440,10 @@
         <v>2</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>1</v>
@@ -7695,13 +7470,13 @@
         <v>1</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="X35" s="1" t="s">
         <v>1</v>
@@ -7758,13 +7533,13 @@
         <v>1</v>
       </c>
       <c r="AP35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AQ35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR35" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AS35" s="1" t="s">
         <v>1</v>
@@ -7821,7 +7596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -7850,16 +7625,16 @@
         <v>2</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>1</v>
@@ -7880,16 +7655,16 @@
         <v>1</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="X36" s="1" t="s">
         <v>1</v>
@@ -7946,13 +7721,13 @@
         <v>1</v>
       </c>
       <c r="AP36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AQ36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR36" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AS36" s="1" t="s">
         <v>2</v>
@@ -8009,7 +7784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -8041,10 +7816,10 @@
         <v>1</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>2</v>
@@ -8068,13 +7843,13 @@
         <v>1</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>1</v>
@@ -8137,7 +7912,7 @@
         <v>1</v>
       </c>
       <c r="AQ37" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AR37" s="1" t="s">
         <v>2</v>
@@ -8197,7 +7972,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -8256,10 +8031,10 @@
         <v>1</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>1</v>
@@ -8385,7 +8160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -8444,10 +8219,10 @@
         <v>1</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>1</v>
@@ -8573,7 +8348,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -8632,10 +8407,10 @@
         <v>1</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>1</v>
@@ -8761,7 +8536,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -8949,7 +8724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -9137,7 +8912,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -9325,7 +9100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -9513,7 +9288,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -9701,7 +9476,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -9889,7 +9664,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -10077,7 +9852,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -10265,7 +10040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -10453,7 +10228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -10641,7 +10416,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -10829,7 +10604,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -11017,7 +10792,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -11205,7 +10980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -11393,7 +11168,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -11581,7 +11356,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -11769,7 +11544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -11957,7 +11732,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -12145,7 +11920,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -12333,7 +12108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -12521,7 +12296,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -12709,7 +12484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -12897,7 +12672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:62" x14ac:dyDescent="0.3">
       <c r="B63" s="5">
         <v>0</v>
       </c>
@@ -13081,27 +12856,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="z">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="z">
       <formula>NOT(ISERROR(SEARCH("z",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="G">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26">
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="68" priority="2" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",P26)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13118,7 +12893,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>